<commit_message>
wrote everything up did second experiment need to do third
</commit_message>
<xml_diff>
--- a/experiment2.xlsx
+++ b/experiment2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Frequency (Hz)</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>∆%</t>
+  </si>
+  <si>
+    <t>gradient</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>∆gradient</t>
+  </si>
+  <si>
+    <t>∆intercept</t>
   </si>
 </sst>
 </file>
@@ -116,6 +128,1159 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Current by Frequency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:backward val="2.7000000000000007E-2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$25:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.26780000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12232000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.7000000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$25:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-686B-44BF-9647-94328440C9F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="262630712"/>
+        <c:axId val="262629400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="262630712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="262629400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="262629400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="262630712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30ED0390-3892-4AF3-97C3-193EE0069C27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98CA700-5E3B-4D32-9FFA-D930D423034D}">
-  <dimension ref="B3:P14"/>
+  <dimension ref="A3:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,12 +1596,12 @@
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -483,12 +1648,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1000</v>
       </c>
       <c r="C5">
-        <f>1/B5</f>
+        <f t="shared" ref="C5:C14" si="0">1/B5</f>
         <v>1E-3</v>
       </c>
       <c r="D5">
@@ -513,11 +1678,11 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="K5">
-        <f>AVERAGE(F5:J5)</f>
+        <f t="shared" ref="K5:K14" si="1">AVERAGE(F5:J5)</f>
         <v>0.26780000000000004</v>
       </c>
       <c r="L5">
-        <f>(K5/100) * 5</f>
+        <f t="shared" ref="L5:L14" si="2">(K5/100) * 5</f>
         <v>1.3390000000000001E-2</v>
       </c>
       <c r="M5">
@@ -528,20 +1693,20 @@
         <v>2.0000000000000017E-4</v>
       </c>
       <c r="O5">
-        <f>(((L5^2)+(M5^2)+(N5^2))^0.5)</f>
+        <f t="shared" ref="O5:O14" si="3">(((L5^2)+(M5^2)+(N5^2))^0.5)</f>
         <v>1.3428778797790961E-2</v>
       </c>
       <c r="P5">
-        <f>(O5/K5)*100</f>
+        <f t="shared" ref="P5:P14" si="4">(O5/K5)*100</f>
         <v>5.0144805070167875</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>900</v>
       </c>
       <c r="C6">
-        <f>1/B6</f>
+        <f t="shared" si="0"/>
         <v>1.1111111111111111E-3</v>
       </c>
       <c r="D6">
@@ -566,11 +1731,11 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="K6">
-        <f>AVERAGE(F6:J6)</f>
+        <f t="shared" si="1"/>
         <v>0.2394</v>
       </c>
       <c r="L6">
-        <f>(K6/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>1.197E-2</v>
       </c>
       <c r="M6">
@@ -581,20 +1746,20 @@
         <v>2.0000000000000017E-4</v>
       </c>
       <c r="O6">
-        <f>(((L6^2)+(M6^2)+(N6^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>1.2013363392489216E-2</v>
       </c>
       <c r="P6">
-        <f>(O6/K6)*100</f>
+        <f t="shared" si="4"/>
         <v>5.0181133636128719</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>800</v>
       </c>
       <c r="C7">
-        <f>1/B7</f>
+        <f t="shared" si="0"/>
         <v>1.25E-3</v>
       </c>
       <c r="D7">
@@ -619,11 +1784,11 @@
         <v>0.21199999999999999</v>
       </c>
       <c r="K7">
-        <f>AVERAGE(F7:J7)</f>
+        <f t="shared" si="1"/>
         <v>0.21259999999999998</v>
       </c>
       <c r="L7">
-        <f>(K7/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>1.0629999999999999E-2</v>
       </c>
       <c r="M7">
@@ -634,20 +1799,20 @@
         <v>2.0000000000000017E-4</v>
       </c>
       <c r="O7">
-        <f>(((L7^2)+(M7^2)+(N7^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>1.0678806113044659E-2</v>
       </c>
       <c r="P7">
-        <f>(O7/K7)*100</f>
+        <f t="shared" si="4"/>
         <v>5.0229567794189371</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>700</v>
       </c>
       <c r="C8">
-        <f>1/B8</f>
+        <f t="shared" si="0"/>
         <v>1.4285714285714286E-3</v>
       </c>
       <c r="D8">
@@ -672,11 +1837,11 @@
         <v>0.186</v>
       </c>
       <c r="K8">
-        <f>AVERAGE(F8:J8)</f>
+        <f t="shared" si="1"/>
         <v>0.186</v>
       </c>
       <c r="L8">
-        <f>(K8/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="M8">
@@ -686,20 +1851,20 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <f>(((L8^2)+(M8^2)+(N8^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>9.3536089291780845E-3</v>
       </c>
       <c r="P8">
-        <f>(O8/K8)*100</f>
+        <f t="shared" si="4"/>
         <v>5.0288220049344545</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>600</v>
       </c>
       <c r="C9">
-        <f>1/B9</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666668E-3</v>
       </c>
       <c r="D9">
@@ -724,11 +1889,11 @@
         <v>0.159</v>
       </c>
       <c r="K9">
-        <f>AVERAGE(F9:J9)</f>
+        <f t="shared" si="1"/>
         <v>0.159</v>
       </c>
       <c r="L9">
-        <f>(K9/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>7.9500000000000005E-3</v>
       </c>
       <c r="M9">
@@ -738,20 +1903,20 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <f>(((L9^2)+(M9^2)+(N9^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>8.0126462545154209E-3</v>
       </c>
       <c r="P9">
-        <f>(O9/K9)*100</f>
+        <f t="shared" si="4"/>
         <v>5.0394001600725913</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>500</v>
       </c>
       <c r="C10">
-        <f>1/B10</f>
+        <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
       <c r="D10">
@@ -776,12 +1941,12 @@
         <v>1.33</v>
       </c>
       <c r="K10">
-        <f>AVERAGE(F10:J10)</f>
-        <v>0.61160000000000003</v>
+        <f>AVERAGE(F10:J10)/5</f>
+        <v>0.12232000000000001</v>
       </c>
       <c r="L10">
-        <f>(K10/100) * 5</f>
-        <v>3.058E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.1159999999999999E-3</v>
       </c>
       <c r="M10">
         <v>1E-3</v>
@@ -791,20 +1956,20 @@
         <v>2.0000000000000017E-4</v>
       </c>
       <c r="O10">
-        <f>(((L10^2)+(M10^2)+(N10^2))^0.5)</f>
-        <v>3.0596999852926757E-2</v>
+        <f t="shared" si="3"/>
+        <v>6.2004399843882041E-3</v>
       </c>
       <c r="P10">
-        <f>(O10/K10)*100</f>
-        <v>5.0027795704589195</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>5.0690320343265229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>400</v>
       </c>
       <c r="C11">
-        <f>1/B11</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="D11">
@@ -829,11 +1994,11 @@
         <v>0.106</v>
       </c>
       <c r="K11">
-        <f>AVERAGE(F11:J11)</f>
+        <f t="shared" si="1"/>
         <v>0.10600000000000001</v>
       </c>
       <c r="L11">
-        <f>(K11/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>5.3000000000000009E-3</v>
       </c>
       <c r="M11">
@@ -843,20 +2008,20 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <f>(((L11^2)+(M11^2)+(N11^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>5.3935146240647212E-3</v>
       </c>
       <c r="P11">
-        <f>(O11/K11)*100</f>
+        <f t="shared" si="4"/>
         <v>5.0882213434572838</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>300</v>
       </c>
       <c r="C12">
-        <f>1/B12</f>
+        <f t="shared" si="0"/>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="D12">
@@ -881,11 +2046,11 @@
         <v>0.08</v>
       </c>
       <c r="K12">
-        <f>AVERAGE(F12:J12)</f>
+        <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
       <c r="L12">
-        <f>(K12/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="M12">
@@ -895,20 +2060,20 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <f>(((L12^2)+(M12^2)+(N12^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>4.1231056256176603E-3</v>
       </c>
       <c r="P12">
-        <f>(O12/K12)*100</f>
+        <f t="shared" si="4"/>
         <v>5.1538820320220751</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>200</v>
       </c>
       <c r="C13">
-        <f>1/B13</f>
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D13">
@@ -933,11 +2098,11 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="K13">
-        <f>AVERAGE(F13:J13)</f>
+        <f t="shared" si="1"/>
         <v>5.3000000000000005E-2</v>
       </c>
       <c r="L13">
-        <f>(K13/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>2.6500000000000004E-3</v>
       </c>
       <c r="M13">
@@ -947,20 +2112,20 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <f>(((L13^2)+(M13^2)+(N13^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>2.83240180765371E-3</v>
       </c>
       <c r="P13">
-        <f>(O13/K13)*100</f>
+        <f t="shared" si="4"/>
         <v>5.344154354063603</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>100</v>
       </c>
       <c r="C14">
-        <f>1/B14</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="D14">
@@ -985,11 +2150,11 @@
         <v>2.7E-2</v>
       </c>
       <c r="K14">
-        <f>AVERAGE(F14:J14)</f>
+        <f t="shared" si="1"/>
         <v>2.7000000000000003E-2</v>
       </c>
       <c r="L14">
-        <f>(K14/100) * 5</f>
+        <f t="shared" si="2"/>
         <v>1.3500000000000003E-3</v>
       </c>
       <c r="M14">
@@ -999,16 +2164,126 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <f>(((L14^2)+(M14^2)+(N14^2))^0.5)</f>
+        <f t="shared" si="3"/>
         <v>1.6800297616411445E-3</v>
       </c>
       <c r="P14">
-        <f>(O14/K14)*100</f>
+        <f t="shared" si="4"/>
         <v>6.2223324505227566</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <f t="array" ref="B16:C17">LINEST(B5:B14,K5:K14,TRUE,TRUE)</f>
+        <v>3733.3100204440184</v>
+      </c>
+      <c r="C16">
+        <v>7.5052543092386941</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>56.173675313844747</v>
+      </c>
+      <c r="C17">
+        <v>9.2343976846657831</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <v>0.26780000000000004</v>
+      </c>
+      <c r="K25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <v>0.2394</v>
+      </c>
+      <c r="K26">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <v>0.21259999999999998</v>
+      </c>
+      <c r="K27">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <v>0.186</v>
+      </c>
+      <c r="K28">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <v>0.159</v>
+      </c>
+      <c r="K29">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>0.12232000000000001</v>
+      </c>
+      <c r="K30">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <v>0.10600000000000001</v>
+      </c>
+      <c r="K31">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>0.08</v>
+      </c>
+      <c r="K32">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>5.3000000000000005E-2</v>
+      </c>
+      <c r="K33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="K34">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>